<commit_message>
Finish odd lot data collection, whew!
</commit_message>
<xml_diff>
--- a/OddLot/data/results-mult-account/mult_appreciation.xlsx
+++ b/OddLot/data/results-mult-account/mult_appreciation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2172F3A-349A-40C5-B5CF-81D0403425EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0B0464-04C8-4952-9102-9038977C36BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="532" windowWidth="16875" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25% Appreciation" sheetId="1" r:id="rId1"/>
@@ -13,10 +13,16 @@
     <sheet name="75% Appreciation" sheetId="3" r:id="rId3"/>
     <sheet name="100% Appreciation" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -351,13 +357,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.3984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -376,13 +383,13 @@
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>3.7386788000000002</v>
+        <v>3.6183943499999902</v>
       </c>
       <c r="D2">
         <v>2000</v>
       </c>
       <c r="E2">
-        <v>373867.88</v>
+        <v>361839.43499999901</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -390,13 +397,13 @@
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>2.3541133448420202</v>
+        <v>0.48308507912495602</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3">
-        <v>1115538.6999999899</v>
+        <v>223107.74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -404,13 +411,13 @@
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>2.0729407952998402</v>
+        <v>1.38285813792866</v>
       </c>
       <c r="D4">
         <v>2002</v>
       </c>
       <c r="E4">
-        <v>3294745.73999999</v>
+        <v>947184.77500000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -418,13 +425,13 @@
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>1.0085237485762899</v>
+        <v>0.63053481623893903</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5">
-        <v>5044738.8312499998</v>
+        <v>1047716.79625</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -432,13 +439,13 @@
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>0.30582105962144701</v>
+        <v>0.25738127612057898</v>
       </c>
       <c r="D6">
         <v>2004</v>
       </c>
       <c r="E6">
-        <v>3127766.4649999999</v>
+        <v>718616.73499999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -446,13 +453,13 @@
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>0.38843138470626298</v>
+        <v>0.35475937604982</v>
       </c>
       <c r="D7">
         <v>2005</v>
       </c>
       <c r="E7">
-        <v>5187581.2474999903</v>
+        <v>1245435.5215</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -460,13 +467,13 @@
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>0.34940432994078402</v>
+        <v>0.323234962186014</v>
       </c>
       <c r="D8">
         <v>2006</v>
       </c>
       <c r="E8">
-        <v>6478930.2324999897</v>
+        <v>1537332.68449999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -474,13 +481,13 @@
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>0.41714421717709799</v>
+        <v>0.39419411588539999</v>
       </c>
       <c r="D9">
         <v>2007</v>
       </c>
       <c r="E9">
-        <v>10437664.8449999</v>
+        <v>2480827.8899999899</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -488,13 +495,13 @@
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>0.10612622127052</v>
+        <v>8.5777645630829194E-2</v>
       </c>
       <c r="D10">
         <v>2008</v>
       </c>
       <c r="E10">
-        <v>3763170.2787500001</v>
+        <v>752634.05574999901</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -502,13 +509,13 @@
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>7.0315731436760703E-2</v>
+        <v>5.8391231411115997E-2</v>
       </c>
       <c r="D11">
         <v>2009</v>
       </c>
       <c r="E11">
-        <v>2896349.8299999898</v>
+        <v>579269.96600000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -516,13 +523,13 @@
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>0.434447151713382</v>
+        <v>0.41095130466015201</v>
       </c>
       <c r="D12">
         <v>2010</v>
       </c>
       <c r="E12">
-        <v>19156181.5275</v>
+        <v>4315406.1294999998</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -530,13 +537,13 @@
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>0.125032620902298</v>
+        <v>0.116563714058132</v>
       </c>
       <c r="D13">
         <v>2011</v>
       </c>
       <c r="E13">
-        <v>7908240.6562499898</v>
+        <v>1727057.1652499901</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -544,13 +551,13 @@
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>0.15232334819031901</v>
+        <v>0.131036198158442</v>
       </c>
       <c r="D14">
         <v>2012</v>
       </c>
       <c r="E14">
-        <v>10838973.002499901</v>
+        <v>2167794.6004999899</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -558,13 +565,13 @@
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>0.201082721127056</v>
+        <v>0.17976861291837501</v>
       </c>
       <c r="D15">
         <v>2013</v>
       </c>
       <c r="E15">
-        <v>16752027.135</v>
+        <v>3410888.9730000002</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -572,13 +579,13 @@
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>0.166459821042239</v>
+        <v>0.15224263048349701</v>
       </c>
       <c r="D16">
         <v>2014</v>
       </c>
       <c r="E16">
-        <v>16656162.789999999</v>
+        <v>3407899.9219999998</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -586,13 +593,13 @@
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>8.0896030844867503E-2</v>
+        <v>7.8045735004012601E-2</v>
       </c>
       <c r="D17">
         <v>2015</v>
       </c>
       <c r="E17">
-        <v>9457315.2499999795</v>
+        <v>2015960.7749999899</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -600,13 +607,13 @@
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>8.7675084908331702E-2</v>
+        <v>7.95720738362415E-2</v>
       </c>
       <c r="D18">
         <v>2016</v>
       </c>
       <c r="E18">
-        <v>11079005.2899999</v>
+        <v>2215801.0580000002</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -614,13 +621,13 @@
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>9.2610167941291802E-2</v>
+        <v>8.4681919201807093E-2</v>
       </c>
       <c r="D19">
         <v>2017</v>
       </c>
       <c r="E19">
-        <v>12728652.4</v>
+        <v>2545730.48</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -628,13 +635,13 @@
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>3.68669601568462E-2</v>
+        <v>3.3957224579987101E-2</v>
       </c>
       <c r="D20">
         <v>2018</v>
       </c>
       <c r="E20">
-        <v>5536385.4974999996</v>
+        <v>1107277.09949999</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +658,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -689,13 +696,13 @@
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>2.2671154554945399</v>
+        <v>0.66144180100000005</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3">
-        <v>661241.63</v>
+        <v>192920.41499999899</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -703,13 +710,13 @@
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>1.15388498154591</v>
+        <v>0.92118750299999996</v>
       </c>
       <c r="D4">
         <v>2002</v>
       </c>
       <c r="E4">
-        <v>1099546.3799999999</v>
+        <v>446395.41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -717,13 +724,13 @@
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>0.80905850566371895</v>
+        <v>0.61716333899999998</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5">
-        <v>1760069.9750000001</v>
+        <v>589750.37874999898</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -731,13 +738,13 @@
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>0.28846918735407101</v>
+        <v>0.27883087499999998</v>
       </c>
       <c r="D6">
         <v>2004</v>
       </c>
       <c r="E6">
-        <v>1135277.54999999</v>
+        <v>437493</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -745,13 +752,13 @@
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>0.48006780943086003</v>
+        <v>0.41300601300000001</v>
       </c>
       <c r="D7">
         <v>2005</v>
       </c>
       <c r="E7">
-        <v>2434328.8250000002</v>
+        <v>828704.57099999895</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -759,13 +766,13 @@
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>0.48266002886190801</v>
+        <v>0.37460496599999998</v>
       </c>
       <c r="D8">
         <v>2006</v>
       </c>
       <c r="E8">
-        <v>3622426.6775000002</v>
+        <v>1062088.9724999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -773,13 +780,13 @@
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>0.448665600979823</v>
+        <v>0.42866700099999999</v>
       </c>
       <c r="D9">
         <v>2007</v>
       </c>
       <c r="E9">
-        <v>4992552.2899999898</v>
+        <v>1670649.4449999901</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -787,13 +794,13 @@
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>0.18580441065856601</v>
+        <v>0.107586485</v>
       </c>
       <c r="D10">
         <v>2008</v>
       </c>
       <c r="E10">
-        <v>2995187.5062500001</v>
+        <v>599037.50124999904</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -801,13 +808,13 @@
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>0.12712057257880699</v>
+        <v>8.1455154000000002E-2</v>
       </c>
       <c r="D11">
         <v>2009</v>
       </c>
       <c r="E11">
-        <v>2632799.5124999899</v>
+        <v>528330.25049999903</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -815,13 +822,13 @@
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>0.42478892621320702</v>
+        <v>0.37907299300000002</v>
       </c>
       <c r="D12">
         <v>2010</v>
       </c>
       <c r="E12">
-        <v>9917837.7799999993</v>
+        <v>2659473.4075000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -829,13 +836,13 @@
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>0.120206129675816</v>
+        <v>9.6299396999999995E-2</v>
       </c>
       <c r="D13">
         <v>2011</v>
       </c>
       <c r="E13">
-        <v>3998719.6712500001</v>
+        <v>931716.16024999996</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -843,13 +850,13 @@
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>0.20608975713204</v>
+        <v>0.14480696700000001</v>
       </c>
       <c r="D14">
         <v>2012</v>
       </c>
       <c r="E14">
-        <v>7679778.5499999896</v>
+        <v>1535955.70999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -857,13 +864,13 @@
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>0.236344804699367</v>
+        <v>0.20766116200000001</v>
       </c>
       <c r="D15">
         <v>2013</v>
       </c>
       <c r="E15">
-        <v>10829087.425000001</v>
+        <v>2557944.091</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -871,13 +878,13 @@
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>0.19142857707432701</v>
+        <v>0.168964279</v>
       </c>
       <c r="D16">
         <v>2014</v>
       </c>
       <c r="E16">
-        <v>10844066.672499901</v>
+        <v>2513481.9324999899</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -885,13 +892,13 @@
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>8.2888538383754998E-2</v>
+        <v>7.5947081E-2</v>
       </c>
       <c r="D17">
         <v>2015</v>
       </c>
       <c r="E17">
-        <v>5607968.7549999896</v>
+        <v>1323166.344</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -899,13 +906,13 @@
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>0.13081237357873901</v>
+        <v>0.10225379</v>
       </c>
       <c r="D18">
         <v>2016</v>
       </c>
       <c r="E18">
-        <v>9583931.18499998</v>
+        <v>1916786.237</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -913,13 +920,13 @@
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>0.11928667312529601</v>
+        <v>9.5660239999999994E-2</v>
       </c>
       <c r="D19">
         <v>2017</v>
       </c>
       <c r="E19">
-        <v>9882739.2999999896</v>
+        <v>1976547.8599999901</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -927,13 +934,13 @@
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>4.7109891891532002E-2</v>
+        <v>4.1981499999999998E-2</v>
       </c>
       <c r="D20">
         <v>2018</v>
       </c>
       <c r="E20">
-        <v>4368565.5149999997</v>
+        <v>950407.21500000299</v>
       </c>
     </row>
   </sheetData>
@@ -949,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5D33F1-0C00-418B-907A-BBA0383A2BCB}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -988,13 +995,13 @@
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>1.2693004482222201</v>
+        <v>0.59493041144237402</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3">
-        <v>257446.78999999899</v>
+        <v>120667.19500000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -1002,13 +1009,13 @@
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>0.60353785622482903</v>
+        <v>0.56146645247341898</v>
       </c>
       <c r="D4">
         <v>2002</v>
       </c>
       <c r="E4">
-        <v>277791.88999999902</v>
+        <v>181630.424999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -1016,13 +1023,13 @@
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>0.50817366154435695</v>
+        <v>0.42544374335795798</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5">
-        <v>409572.97499999899</v>
+        <v>223325.35499999899</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -1030,13 +1037,13 @@
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>0.435334737289711</v>
+        <v>0.37743068997359602</v>
       </c>
       <c r="D6">
         <v>2004</v>
       </c>
       <c r="E6">
-        <v>529168.29500000004</v>
+        <v>282412.02500000002</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1044,13 +1051,13 @@
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>0.55043740577526701</v>
+        <v>0.48863710951711498</v>
       </c>
       <c r="D7">
         <v>2005</v>
       </c>
       <c r="E7">
-        <v>960354.61499999999</v>
+        <v>503619.08</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -1058,13 +1065,13 @@
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>0.47030932466490699</v>
+        <v>0.36419634564571302</v>
       </c>
       <c r="D8">
         <v>2006</v>
       </c>
       <c r="E8">
-        <v>1272217.94</v>
+        <v>558779.1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -1072,13 +1079,13 @@
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>0.44522798214892001</v>
+        <v>0.38487222034280899</v>
       </c>
       <c r="D9">
         <v>2007</v>
       </c>
       <c r="E9">
-        <v>1770798.27</v>
+        <v>805560.23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -1086,13 +1093,13 @@
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>0.31391276300704002</v>
+        <v>0.17883225156996599</v>
       </c>
       <c r="D10">
         <v>2008</v>
       </c>
       <c r="E10">
-        <v>1804396.4862500001</v>
+        <v>518366.58724999899</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -1100,13 +1107,13 @@
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>0.223616381256171</v>
+        <v>0.1218766922108</v>
       </c>
       <c r="D11">
         <v>2009</v>
       </c>
       <c r="E11">
-        <v>1872083.19749999</v>
+        <v>446271.80949999898</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -1114,13 +1121,13 @@
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>0.31443076897578498</v>
+        <v>0.29000947116618597</v>
       </c>
       <c r="D12">
         <v>2010</v>
       </c>
       <c r="E12">
-        <v>3221008.37</v>
+        <v>1191341.04999999</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -1128,13 +1135,13 @@
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>8.9679799891598494E-2</v>
+        <v>7.2225492514558898E-2</v>
       </c>
       <c r="D13">
         <v>2011</v>
       </c>
       <c r="E13">
-        <v>1207533.4299999899</v>
+        <v>382743.06999999902</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -1142,13 +1149,13 @@
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>0.19163297968427401</v>
+        <v>0.13874159154784799</v>
       </c>
       <c r="D14">
         <v>2012</v>
       </c>
       <c r="E14">
-        <v>2811730.4550000001</v>
+        <v>788332.85099999898</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -1156,13 +1163,13 @@
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>0.194043728310582</v>
+        <v>0.19499020082483101</v>
       </c>
       <c r="D15">
         <v>2013</v>
       </c>
       <c r="E15">
-        <v>3477594.8999999901</v>
+        <v>1278717.5404999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -1170,13 +1177,13 @@
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>0.25876762317563401</v>
+        <v>0.179476945666351</v>
       </c>
       <c r="D16">
         <v>2014</v>
       </c>
       <c r="E16">
-        <v>5537446.5649999902</v>
+        <v>1406484.17499999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -1184,13 +1191,13 @@
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>0.16142634292348801</v>
+        <v>0.13506998322011601</v>
       </c>
       <c r="D17">
         <v>2015</v>
       </c>
       <c r="E17">
-        <v>4370808.2437499901</v>
+        <v>1252226.0847499899</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -1198,13 +1205,13 @@
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>0.235163955628403</v>
+        <v>0.152712883947942</v>
       </c>
       <c r="D18">
         <v>2016</v>
       </c>
       <c r="E18">
-        <v>7395197.4574999996</v>
+        <v>1607023.4645</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -1212,13 +1219,13 @@
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>0.178458473663484</v>
+        <v>0.142367894437082</v>
       </c>
       <c r="D19">
         <v>2017</v>
       </c>
       <c r="E19">
-        <v>6931716.6500000004</v>
+        <v>1726949.94</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -1226,13 +1233,13 @@
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>6.1981718211891398E-2</v>
+        <v>4.7307926743142499E-2</v>
       </c>
       <c r="D20">
         <v>2018</v>
       </c>
       <c r="E20">
-        <v>2837144.9349999898</v>
+        <v>655552.67099999997</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1256,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E20"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1287,13 +1294,13 @@
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>0.59315239165505096</v>
+        <v>0.496576809614165</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3">
-        <v>94222.25</v>
+        <v>78881.22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -1301,13 +1308,13 @@
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>0.30688253586093101</v>
+        <v>0.27033682567737699</v>
       </c>
       <c r="D4">
         <v>2002</v>
       </c>
       <c r="E4">
-        <v>77663.45</v>
+        <v>64267.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -1315,13 +1322,13 @@
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>0.34923570069011101</v>
+        <v>0.31979248685106998</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5">
-        <v>123379.799999999</v>
+        <v>101373.80499999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -1329,13 +1336,13 @@
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>0.49383735154241798</v>
+        <v>0.45814422380342201</v>
       </c>
       <c r="D6">
         <v>2004</v>
       </c>
       <c r="E6">
-        <v>235394.97500000001</v>
+        <v>191674.95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1343,13 +1350,13 @@
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>0.53028845165550198</v>
+        <v>0.41043141786693299</v>
       </c>
       <c r="D7">
         <v>2005</v>
       </c>
       <c r="E7">
-        <v>377597.17499999999</v>
+        <v>250382.64499999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -1357,13 +1364,13 @@
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>0.54627489649238403</v>
+        <v>0.36899248089130798</v>
       </c>
       <c r="D8">
         <v>2006</v>
       </c>
       <c r="E8">
-        <v>595252.34</v>
+        <v>317492.24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -1371,13 +1378,13 @@
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>0.43428920946288602</v>
+        <v>0.35892346884946003</v>
       </c>
       <c r="D9">
         <v>2007</v>
       </c>
       <c r="E9">
-        <v>731738.00499999896</v>
+        <v>422783.97499999899</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -1385,13 +1392,13 @@
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>0.51383208100977096</v>
+        <v>0.26235243020351001</v>
       </c>
       <c r="D10">
         <v>2008</v>
       </c>
       <c r="E10">
-        <v>1241751.0049999999</v>
+        <v>419949.19374999899</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -1399,13 +1406,13 @@
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>0.30863977021801697</v>
+        <v>0.167926577316208</v>
       </c>
       <c r="D11">
         <v>2009</v>
       </c>
       <c r="E11">
-        <v>1206113.1999999899</v>
+        <v>362457.31999999902</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -1413,13 +1420,13 @@
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>0.28652615791278602</v>
+        <v>0.27364329227853801</v>
       </c>
       <c r="D12">
         <v>2010</v>
       </c>
       <c r="E12">
-        <v>1465279.85</v>
+        <v>689823.18500000006</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -1427,13 +1434,13 @@
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>0.11819712539067501</v>
+        <v>8.8275281142178599E-2</v>
       </c>
       <c r="D13">
         <v>2011</v>
       </c>
       <c r="E13">
-        <v>777645.80999999901</v>
+        <v>283426.13999999902</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -1441,13 +1448,13 @@
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>0.136818280715645</v>
+        <v>7.5595795596146903E-2</v>
       </c>
       <c r="D14">
         <v>2012</v>
       </c>
       <c r="E14">
-        <v>1006554.79499999</v>
+        <v>264141.840499999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -1455,13 +1462,13 @@
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>0.19390952331976199</v>
+        <v>0.18310055651704599</v>
       </c>
       <c r="D15">
         <v>2013</v>
       </c>
       <c r="E15">
-        <v>1621748.4099999899</v>
+        <v>688142.4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -1469,13 +1476,13 @@
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>0.234283684684335</v>
+        <v>0.209911511840492</v>
       </c>
       <c r="D16">
         <v>2014</v>
       </c>
       <c r="E16">
-        <v>2339364.0099999998</v>
+        <v>933354.37749999994</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -1483,13 +1490,13 @@
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>0.237744167664596</v>
+        <v>0.194194725827222</v>
       </c>
       <c r="D17">
         <v>2015</v>
       </c>
       <c r="E17">
-        <v>2930087.6937499898</v>
+        <v>1044723.47074999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -1497,13 +1504,13 @@
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>0.28161752521302902</v>
+        <v>0.19492697189901001</v>
       </c>
       <c r="D18">
         <v>2016</v>
       </c>
       <c r="E18">
-        <v>4295970.7237499896</v>
+        <v>1252307.57075</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -1511,13 +1518,13 @@
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>0.115051447030545</v>
+        <v>0.11055851190174799</v>
       </c>
       <c r="D19">
         <v>2017</v>
       </c>
       <c r="E19">
-        <v>2249324.73</v>
+        <v>848735.99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -1525,13 +1532,13 @@
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>0.14622991945029901</v>
+        <v>0.12164736588753999</v>
       </c>
       <c r="D20">
         <v>2018</v>
       </c>
       <c r="E20">
-        <v>3187801.1224999898</v>
+        <v>1037109.44249999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>